<commit_message>
Moved references to the end
</commit_message>
<xml_diff>
--- a/20230214_Anlagen_Ausschreibung_CZS_Forschungsstart_filled.xlsx
+++ b/20230214_Anlagen_Ausschreibung_CZS_Forschungsstart_filled.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Anlage 1 Meilensteinplan" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="84">
   <si>
     <t xml:space="preserve">Anlage 1</t>
   </si>
@@ -33,10 +33,19 @@
     <t xml:space="preserve">Antragstellende Institution:</t>
   </si>
   <si>
+    <t xml:space="preserve">Technische Hochschule Bingen</t>
+  </si>
+  <si>
     <t xml:space="preserve">Projektname:</t>
   </si>
   <si>
+    <t xml:space="preserve">EasyVectorOmics</t>
+  </si>
+  <si>
     <t xml:space="preserve">Geplanter Projektstart*:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01.11.2023</t>
   </si>
   <si>
     <r>
@@ -349,7 +358,7 @@
     <numFmt numFmtId="165" formatCode="General"/>
     <numFmt numFmtId="166" formatCode="0%"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -399,6 +408,13 @@
       <b val="true"/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -1116,18 +1132,18 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="6" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1188,6 +1204,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="8" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="9" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1240,10 +1260,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1252,7 +1268,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1280,7 +1296,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1304,15 +1320,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="11" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="11" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="11" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="11" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1408,23 +1424,23 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="10" borderId="44" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="10" borderId="44" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="10" borderId="45" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="10" borderId="45" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="10" borderId="46" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="10" borderId="46" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="10" borderId="47" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="10" borderId="47" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="10" borderId="48" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="10" borderId="48" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1468,19 +1484,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="10" borderId="45" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="10" borderId="45" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="10" borderId="48" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="10" borderId="48" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="10" borderId="47" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="10" borderId="47" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="10" borderId="52" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="10" borderId="52" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1488,11 +1504,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1552,23 +1568,23 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="10" borderId="60" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="10" borderId="60" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="10" borderId="61" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="10" borderId="61" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="10" borderId="62" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="10" borderId="62" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="10" borderId="63" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="10" borderId="63" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="10" borderId="64" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="10" borderId="64" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1616,7 +1632,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1731,9 +1747,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>40</xdr:col>
-      <xdr:colOff>38160</xdr:colOff>
+      <xdr:colOff>37800</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>180720</xdr:rowOff>
+      <xdr:rowOff>180360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1747,7 +1763,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10437120" y="106200"/>
-          <a:ext cx="1955520" cy="1095120"/>
+          <a:ext cx="1955160" cy="1094760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1768,9 +1784,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>40</xdr:col>
-      <xdr:colOff>5760</xdr:colOff>
+      <xdr:colOff>5400</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>190080</xdr:rowOff>
+      <xdr:rowOff>189720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1784,7 +1800,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10437120" y="106200"/>
-          <a:ext cx="1923120" cy="1104480"/>
+          <a:ext cx="1922760" cy="1104120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1810,9 +1826,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>2987280</xdr:colOff>
+      <xdr:colOff>2986920</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>19800</xdr:rowOff>
+      <xdr:rowOff>19440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1825,8 +1841,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12663000" y="177840"/>
-          <a:ext cx="1971360" cy="1118160"/>
+          <a:off x="12662280" y="177840"/>
+          <a:ext cx="1971000" cy="1117800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1848,8 +1864,8 @@
   </sheetPr>
   <dimension ref="B2:AN24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="X34" activeCellId="0" sqref="X34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S7" activeCellId="0" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.57421875" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1881,20 +1897,29 @@
       <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="D6" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -1974,84 +1999,84 @@
     </row>
     <row r="14" s="6" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="9" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
       <c r="H14" s="12" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="I14" s="12"/>
       <c r="J14" s="12"/>
       <c r="K14" s="12" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="L14" s="12"/>
       <c r="M14" s="12"/>
       <c r="N14" s="12" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="O14" s="12"/>
       <c r="P14" s="12"/>
       <c r="Q14" s="12" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="R14" s="12"/>
       <c r="S14" s="12"/>
       <c r="T14" s="12" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="U14" s="12"/>
       <c r="V14" s="12"/>
       <c r="W14" s="12" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="X14" s="12"/>
       <c r="Y14" s="12"/>
       <c r="Z14" s="12" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="AA14" s="12"/>
       <c r="AB14" s="12"/>
       <c r="AC14" s="12" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="AD14" s="12"/>
       <c r="AE14" s="12"/>
       <c r="AF14" s="12" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="AG14" s="12"/>
       <c r="AH14" s="12"/>
       <c r="AI14" s="12" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="AJ14" s="12"/>
       <c r="AK14" s="12"/>
       <c r="AL14" s="12" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="AM14" s="12"/>
       <c r="AN14" s="12"/>
     </row>
     <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="13" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E15" s="16"/>
       <c r="F15" s="17"/>
@@ -2062,10 +2087,10 @@
       <c r="K15" s="16"/>
       <c r="L15" s="17"/>
       <c r="M15" s="18"/>
-      <c r="N15" s="19"/>
-      <c r="O15" s="20"/>
-      <c r="P15" s="21"/>
-      <c r="Q15" s="19"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="19"/>
+      <c r="P15" s="20"/>
+      <c r="Q15" s="21"/>
       <c r="R15" s="17"/>
       <c r="S15" s="18"/>
       <c r="T15" s="16"/>
@@ -2092,13 +2117,13 @@
     </row>
     <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="22" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E16" s="25"/>
       <c r="F16" s="26"/>
@@ -2115,7 +2140,7 @@
       <c r="Q16" s="28"/>
       <c r="R16" s="29"/>
       <c r="S16" s="30"/>
-      <c r="T16" s="25"/>
+      <c r="T16" s="28"/>
       <c r="U16" s="26"/>
       <c r="V16" s="27"/>
       <c r="W16" s="25"/>
@@ -2139,13 +2164,13 @@
     </row>
     <row r="17" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="24" t="s">
         <v>18</v>
-      </c>
-      <c r="C17" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="24" t="s">
-        <v>15</v>
       </c>
       <c r="E17" s="25"/>
       <c r="F17" s="26"/>
@@ -2165,7 +2190,7 @@
       <c r="T17" s="31"/>
       <c r="U17" s="32"/>
       <c r="V17" s="33"/>
-      <c r="W17" s="25"/>
+      <c r="W17" s="31"/>
       <c r="X17" s="26"/>
       <c r="Y17" s="27"/>
       <c r="Z17" s="25"/>
@@ -2186,13 +2211,13 @@
     </row>
     <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="22" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D18" s="24" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E18" s="25"/>
       <c r="F18" s="26"/>
@@ -2216,7 +2241,7 @@
       <c r="X18" s="32"/>
       <c r="Y18" s="33"/>
       <c r="Z18" s="31"/>
-      <c r="AA18" s="26"/>
+      <c r="AA18" s="32"/>
       <c r="AB18" s="27"/>
       <c r="AC18" s="25"/>
       <c r="AD18" s="26"/>
@@ -2233,13 +2258,13 @@
     </row>
     <row r="19" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="22" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E19" s="25"/>
       <c r="F19" s="26"/>
@@ -2269,7 +2294,7 @@
       <c r="AD19" s="34"/>
       <c r="AE19" s="35"/>
       <c r="AF19" s="36"/>
-      <c r="AG19" s="26"/>
+      <c r="AG19" s="37"/>
       <c r="AH19" s="27"/>
       <c r="AI19" s="25"/>
       <c r="AJ19" s="26"/>
@@ -2280,13 +2305,13 @@
     </row>
     <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="22" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E20" s="25"/>
       <c r="F20" s="26"/>
@@ -2316,12 +2341,12 @@
       <c r="AD20" s="26"/>
       <c r="AE20" s="27"/>
       <c r="AF20" s="25"/>
-      <c r="AG20" s="37"/>
-      <c r="AH20" s="38"/>
-      <c r="AI20" s="39"/>
-      <c r="AJ20" s="37"/>
-      <c r="AK20" s="38"/>
-      <c r="AL20" s="25"/>
+      <c r="AG20" s="38"/>
+      <c r="AH20" s="39"/>
+      <c r="AI20" s="40"/>
+      <c r="AJ20" s="38"/>
+      <c r="AK20" s="39"/>
+      <c r="AL20" s="40"/>
       <c r="AM20" s="26"/>
       <c r="AN20" s="27"/>
     </row>
@@ -2449,45 +2474,45 @@
       <c r="AN23" s="27"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="40"/>
-      <c r="C24" s="41"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="43"/>
-      <c r="F24" s="44"/>
-      <c r="G24" s="45"/>
-      <c r="H24" s="43"/>
-      <c r="I24" s="44"/>
-      <c r="J24" s="45"/>
-      <c r="K24" s="43"/>
-      <c r="L24" s="44"/>
-      <c r="M24" s="45"/>
-      <c r="N24" s="43"/>
-      <c r="O24" s="44"/>
-      <c r="P24" s="45"/>
-      <c r="Q24" s="43"/>
-      <c r="R24" s="44"/>
-      <c r="S24" s="45"/>
-      <c r="T24" s="43"/>
-      <c r="U24" s="44"/>
-      <c r="V24" s="45"/>
-      <c r="W24" s="43"/>
-      <c r="X24" s="44"/>
-      <c r="Y24" s="45"/>
-      <c r="Z24" s="43"/>
-      <c r="AA24" s="44"/>
-      <c r="AB24" s="45"/>
-      <c r="AC24" s="43"/>
-      <c r="AD24" s="44"/>
-      <c r="AE24" s="45"/>
-      <c r="AF24" s="43"/>
-      <c r="AG24" s="44"/>
-      <c r="AH24" s="45"/>
-      <c r="AI24" s="43"/>
-      <c r="AJ24" s="44"/>
-      <c r="AK24" s="45"/>
-      <c r="AL24" s="43"/>
-      <c r="AM24" s="44"/>
-      <c r="AN24" s="45"/>
+      <c r="B24" s="41"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="44"/>
+      <c r="F24" s="45"/>
+      <c r="G24" s="46"/>
+      <c r="H24" s="44"/>
+      <c r="I24" s="45"/>
+      <c r="J24" s="46"/>
+      <c r="K24" s="44"/>
+      <c r="L24" s="45"/>
+      <c r="M24" s="46"/>
+      <c r="N24" s="44"/>
+      <c r="O24" s="45"/>
+      <c r="P24" s="46"/>
+      <c r="Q24" s="44"/>
+      <c r="R24" s="45"/>
+      <c r="S24" s="46"/>
+      <c r="T24" s="44"/>
+      <c r="U24" s="45"/>
+      <c r="V24" s="46"/>
+      <c r="W24" s="44"/>
+      <c r="X24" s="45"/>
+      <c r="Y24" s="46"/>
+      <c r="Z24" s="44"/>
+      <c r="AA24" s="45"/>
+      <c r="AB24" s="46"/>
+      <c r="AC24" s="44"/>
+      <c r="AD24" s="45"/>
+      <c r="AE24" s="46"/>
+      <c r="AF24" s="44"/>
+      <c r="AG24" s="45"/>
+      <c r="AH24" s="46"/>
+      <c r="AI24" s="44"/>
+      <c r="AJ24" s="45"/>
+      <c r="AK24" s="46"/>
+      <c r="AL24" s="44"/>
+      <c r="AM24" s="45"/>
+      <c r="AN24" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="16">
@@ -2526,74 +2551,83 @@
   </sheetPr>
   <dimension ref="A1:N65"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B35" activeCellId="0" sqref="B35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6015625" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="46" width="5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="46" width="27.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="3" style="46" width="8.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="46" width="15.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="46" width="33.6"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="14" style="46" width="11.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="47" width="5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="47" width="27.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="3" style="47" width="8.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="47" width="15.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="47" width="33.6"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="14" style="47" width="11.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F1" s="47"/>
-      <c r="J1" s="47"/>
+      <c r="F1" s="48"/>
+      <c r="J1" s="48"/>
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="48" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="47"/>
-      <c r="J2" s="47"/>
+      <c r="B2" s="49" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="48"/>
+      <c r="J2" s="48"/>
     </row>
     <row r="3" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F3" s="47"/>
-      <c r="J3" s="47"/>
+      <c r="F3" s="48"/>
+      <c r="J3" s="48"/>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="49" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="47"/>
-      <c r="J4" s="47"/>
+      <c r="B4" s="50" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="48"/>
+      <c r="J4" s="48"/>
     </row>
     <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F5" s="47"/>
-      <c r="J5" s="47"/>
+      <c r="F5" s="48"/>
+      <c r="J5" s="48"/>
     </row>
     <row r="6" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="47"/>
-      <c r="J6" s="47"/>
+      <c r="C6" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="48"/>
+      <c r="J6" s="48"/>
     </row>
     <row r="7" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="48" t="s">
-        <v>3</v>
-      </c>
-      <c r="F7" s="47"/>
-      <c r="J7" s="47"/>
+      <c r="B7" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="48"/>
+      <c r="J7" s="48"/>
     </row>
     <row r="8" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" s="47"/>
-      <c r="J8" s="47"/>
+      <c r="B8" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="47" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="48"/>
+      <c r="J8" s="48"/>
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F9" s="47"/>
-      <c r="J9" s="47"/>
+      <c r="F9" s="48"/>
+      <c r="J9" s="48"/>
     </row>
     <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="51" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C10" s="51"/>
       <c r="D10" s="51"/>
@@ -2605,25 +2639,25 @@
       <c r="J10" s="51"/>
     </row>
     <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F11" s="47"/>
-      <c r="J11" s="47"/>
+      <c r="F11" s="48"/>
+      <c r="J11" s="48"/>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F12" s="47"/>
-      <c r="J12" s="47"/>
+      <c r="F12" s="48"/>
+      <c r="J12" s="48"/>
     </row>
     <row r="13" s="52" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B13" s="53" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
       <c r="G13" s="8" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H13" s="8"/>
       <c r="I13" s="8"/>
@@ -2634,75 +2668,75 @@
     <row r="14" s="52" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="53"/>
       <c r="C14" s="56" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D14" s="56"/>
       <c r="E14" s="57" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F14" s="57"/>
       <c r="G14" s="58" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="H14" s="58"/>
       <c r="I14" s="57" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="J14" s="57"/>
       <c r="K14" s="59" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="L14" s="59"/>
       <c r="M14" s="60" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="N14" s="55"/>
     </row>
     <row r="15" s="52" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="61" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="62" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="63" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="64" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="64" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="65" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" s="63" t="s">
+        <v>41</v>
+      </c>
+      <c r="H15" s="64" t="s">
+        <v>42</v>
+      </c>
+      <c r="I15" s="64" t="s">
+        <v>41</v>
+      </c>
+      <c r="J15" s="65" t="s">
+        <v>42</v>
+      </c>
+      <c r="K15" s="66" t="s">
+        <v>35</v>
+      </c>
+      <c r="L15" s="67" t="s">
         <v>36</v>
-      </c>
-      <c r="B15" s="62" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="63" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="64" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" s="64" t="s">
-        <v>38</v>
-      </c>
-      <c r="F15" s="65" t="s">
-        <v>39</v>
-      </c>
-      <c r="G15" s="63" t="s">
-        <v>38</v>
-      </c>
-      <c r="H15" s="64" t="s">
-        <v>39</v>
-      </c>
-      <c r="I15" s="64" t="s">
-        <v>38</v>
-      </c>
-      <c r="J15" s="65" t="s">
-        <v>39</v>
-      </c>
-      <c r="K15" s="66" t="s">
-        <v>32</v>
-      </c>
-      <c r="L15" s="67" t="s">
-        <v>33</v>
       </c>
       <c r="M15" s="68"/>
     </row>
     <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="61" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B16" s="69" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C16" s="70"/>
       <c r="D16" s="71"/>
@@ -2729,14 +2763,14 @@
         <v>138000</v>
       </c>
       <c r="M16" s="76"/>
-      <c r="N16" s="47"/>
+      <c r="N16" s="48"/>
     </row>
     <row r="17" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="61" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B17" s="77" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C17" s="78"/>
       <c r="D17" s="79"/>
@@ -2766,7 +2800,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="61" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B18" s="77"/>
       <c r="C18" s="78"/>
@@ -2786,11 +2820,11 @@
         <v>0</v>
       </c>
       <c r="M18" s="77"/>
-      <c r="N18" s="47"/>
+      <c r="N18" s="48"/>
     </row>
     <row r="19" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="61" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B19" s="69"/>
       <c r="C19" s="82"/>
@@ -2810,11 +2844,11 @@
         <v>0</v>
       </c>
       <c r="M19" s="77"/>
-      <c r="N19" s="47"/>
+      <c r="N19" s="48"/>
     </row>
     <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="61" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B20" s="77"/>
       <c r="C20" s="78"/>
@@ -2834,11 +2868,11 @@
         <v>0</v>
       </c>
       <c r="M20" s="77"/>
-      <c r="N20" s="47"/>
+      <c r="N20" s="48"/>
     </row>
     <row r="21" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="61" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B21" s="69"/>
       <c r="C21" s="82"/>
@@ -2858,11 +2892,11 @@
         <v>0</v>
       </c>
       <c r="M21" s="69"/>
-      <c r="N21" s="47"/>
+      <c r="N21" s="48"/>
     </row>
     <row r="22" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="61" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B22" s="84"/>
       <c r="C22" s="70"/>
@@ -2882,12 +2916,12 @@
         <v>0</v>
       </c>
       <c r="M22" s="90"/>
-      <c r="N22" s="47"/>
+      <c r="N22" s="48"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="91"/>
       <c r="B23" s="92" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C23" s="93" t="n">
         <f aca="false">SUM(C16:C22)</f>
@@ -2934,35 +2968,35 @@
     <row r="24" s="52" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="61"/>
       <c r="B24" s="62" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C24" s="98" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D24" s="98"/>
       <c r="E24" s="99" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F24" s="99"/>
       <c r="G24" s="98" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="H24" s="98"/>
       <c r="I24" s="99" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="J24" s="99"/>
       <c r="K24" s="66" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="L24" s="67" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="M24" s="100"/>
     </row>
     <row r="25" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="61" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B25" s="69"/>
       <c r="C25" s="101"/>
@@ -2982,11 +3016,11 @@
         <v>0</v>
       </c>
       <c r="M25" s="76"/>
-      <c r="N25" s="47"/>
+      <c r="N25" s="48"/>
     </row>
     <row r="26" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="61" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B26" s="90"/>
       <c r="C26" s="103"/>
@@ -3009,7 +3043,7 @@
     </row>
     <row r="27" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="61" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B27" s="90"/>
       <c r="C27" s="103"/>
@@ -3032,7 +3066,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="61" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B28" s="90"/>
       <c r="C28" s="103"/>
@@ -3052,11 +3086,11 @@
         <v>0</v>
       </c>
       <c r="M28" s="90"/>
-      <c r="N28" s="47"/>
+      <c r="N28" s="48"/>
     </row>
     <row r="29" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="61" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B29" s="90"/>
       <c r="C29" s="103"/>
@@ -3076,11 +3110,11 @@
         <v>0</v>
       </c>
       <c r="M29" s="90"/>
-      <c r="N29" s="47"/>
+      <c r="N29" s="48"/>
     </row>
     <row r="30" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="61" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B30" s="90"/>
       <c r="C30" s="103"/>
@@ -3100,11 +3134,11 @@
         <v>0</v>
       </c>
       <c r="M30" s="90"/>
-      <c r="N30" s="47"/>
+      <c r="N30" s="48"/>
     </row>
     <row r="31" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="61" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B31" s="84"/>
       <c r="C31" s="87"/>
@@ -3124,12 +3158,12 @@
         <v>0</v>
       </c>
       <c r="M31" s="84"/>
-      <c r="N31" s="47"/>
+      <c r="N31" s="48"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="91"/>
       <c r="B32" s="92" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C32" s="107" t="n">
         <f aca="false">SUM(C25:D31)</f>
@@ -3160,43 +3194,43 @@
         <v>0</v>
       </c>
       <c r="M32" s="111"/>
-      <c r="N32" s="47"/>
+      <c r="N32" s="48"/>
     </row>
     <row r="33" s="52" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="61"/>
       <c r="B33" s="62" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C33" s="98" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D33" s="98"/>
       <c r="E33" s="99" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F33" s="99"/>
       <c r="G33" s="98" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="H33" s="98"/>
       <c r="I33" s="99" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="J33" s="99"/>
       <c r="K33" s="112" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="L33" s="113" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="M33" s="114"/>
     </row>
     <row r="34" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="61" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B34" s="69" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C34" s="115"/>
       <c r="D34" s="115"/>
@@ -3220,7 +3254,7 @@
     </row>
     <row r="35" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="61" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B35" s="120"/>
       <c r="C35" s="121"/>
@@ -3243,7 +3277,7 @@
     </row>
     <row r="36" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="61" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B36" s="123"/>
       <c r="C36" s="103"/>
@@ -3266,7 +3300,7 @@
     </row>
     <row r="37" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="61" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B37" s="123"/>
       <c r="C37" s="103"/>
@@ -3289,7 +3323,7 @@
     </row>
     <row r="38" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="61" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B38" s="123"/>
       <c r="C38" s="103"/>
@@ -3312,7 +3346,7 @@
     </row>
     <row r="39" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="61" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B39" s="123"/>
       <c r="C39" s="103"/>
@@ -3335,7 +3369,7 @@
     </row>
     <row r="40" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="61" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B40" s="125"/>
       <c r="C40" s="87"/>
@@ -3358,7 +3392,7 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="128" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C41" s="129" t="n">
         <f aca="false">SUM(C34:D40)</f>
@@ -3389,11 +3423,11 @@
         <v>5000</v>
       </c>
       <c r="M41" s="133"/>
-      <c r="N41" s="47"/>
+      <c r="N41" s="48"/>
     </row>
     <row r="42" s="52" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B42" s="134" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C42" s="135" t="n">
         <f aca="false">SUM(D23+C32+C41)</f>
@@ -3426,7 +3460,7 @@
     </row>
     <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L43" s="140"/>
-      <c r="M43" s="47"/>
+      <c r="M43" s="48"/>
     </row>
     <row r="44" s="52" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K44" s="141" t="n">
@@ -3448,7 +3482,7 @@
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="48" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B48" s="144" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C48" s="144"/>
       <c r="D48" s="144"/>
@@ -3809,89 +3843,89 @@
   </sheetPr>
   <dimension ref="A2:C12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6015625" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="46" width="2.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="46" width="14.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="46" width="47"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="46" width="11.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="47" width="2.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="47" width="14.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="47" width="47"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="47" width="11.6"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="49" t="s">
-        <v>66</v>
+      <c r="B2" s="50" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="49"/>
+      <c r="B3" s="50"/>
     </row>
     <row r="5" s="52" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B5" s="145" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C5" s="145" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="146" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C6" s="147" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="54.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="146" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C7" s="147" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="96" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="146" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C8" s="147" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="54.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="146" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C9" s="147" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="54.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="148"/>
       <c r="B10" s="149" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C10" s="150" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="149" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C11" s="151" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="149" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C12" s="150" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>